<commit_message>
Updated components and added new files
</commit_message>
<xml_diff>
--- a/backend-contact-form/contacts.xlsx
+++ b/backend-contact-form/contacts.xlsx
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -613,9 +613,285 @@
         <v>hi i waant to meet u</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>AEDAKULA</v>
+      </c>
+      <c r="B10" t="str">
+        <v/>
+      </c>
+      <c r="C10" t="str">
+        <v/>
+      </c>
+      <c r="D10" t="str">
+        <v>rithvikanirvesh2909@gmail.com</v>
+      </c>
+      <c r="E10" t="str">
+        <v>8125577708</v>
+      </c>
+      <c r="F10" t="str">
+        <v>IT Consulting</v>
+      </c>
+      <c r="G10" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>a.bobby</v>
+      </c>
+      <c r="B11" t="str">
+        <v/>
+      </c>
+      <c r="C11" t="str">
+        <v>beb</v>
+      </c>
+      <c r="D11" t="str">
+        <v>rithvikanirvesh2909@gmail.com</v>
+      </c>
+      <c r="E11" t="str">
+        <v>8125577708</v>
+      </c>
+      <c r="F11" t="str">
+        <v>Managed Services</v>
+      </c>
+      <c r="G11" t="str">
+        <v>gggg</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>bhanu</v>
+      </c>
+      <c r="B12" t="str">
+        <v>annna</v>
+      </c>
+      <c r="C12" t="str">
+        <v>beb</v>
+      </c>
+      <c r="D12" t="str">
+        <v>rithvikanirvesh2909@gmail.com</v>
+      </c>
+      <c r="E12" t="str">
+        <v/>
+      </c>
+      <c r="F12" t="str">
+        <v>Mobile Development</v>
+      </c>
+      <c r="G12" t="str">
+        <v>jjjjj</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Mouli</v>
+      </c>
+      <c r="B13" t="str">
+        <v/>
+      </c>
+      <c r="C13" t="str">
+        <v>mlrit</v>
+      </c>
+      <c r="D13" t="str">
+        <v>rithvikanirvesh0416@gmail.com</v>
+      </c>
+      <c r="E13" t="str">
+        <v>9876543219</v>
+      </c>
+      <c r="F13" t="str">
+        <v>Mobile Development</v>
+      </c>
+      <c r="G13" t="str">
+        <v>haa</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>priya</v>
+      </c>
+      <c r="B14" t="str">
+        <v>chilukiri</v>
+      </c>
+      <c r="C14" t="str">
+        <v>NGO</v>
+      </c>
+      <c r="D14" t="str">
+        <v>priya.chilukuri1122@gmail.com</v>
+      </c>
+      <c r="E14" t="str">
+        <v>9550668312</v>
+      </c>
+      <c r="F14" t="str">
+        <v>Cloud Services</v>
+      </c>
+      <c r="G14" t="str">
+        <v>want an ngo website build for me</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>AEDAKULA</v>
+      </c>
+      <c r="B15" t="str">
+        <v/>
+      </c>
+      <c r="C15" t="str">
+        <v/>
+      </c>
+      <c r="D15" t="str">
+        <v>rithvikanirvesh2909@gmail.com</v>
+      </c>
+      <c r="E15" t="str">
+        <v>08125577708</v>
+      </c>
+      <c r="F15" t="str">
+        <v/>
+      </c>
+      <c r="G15" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>AEDAKULA</v>
+      </c>
+      <c r="B16" t="str">
+        <v/>
+      </c>
+      <c r="C16" t="str">
+        <v/>
+      </c>
+      <c r="D16" t="str">
+        <v>rithvikanirvesh2909@gmail.com</v>
+      </c>
+      <c r="E16" t="str">
+        <v>08125577708</v>
+      </c>
+      <c r="F16" t="str">
+        <v/>
+      </c>
+      <c r="G16" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>AEDAKULA</v>
+      </c>
+      <c r="B17" t="str">
+        <v/>
+      </c>
+      <c r="C17" t="str">
+        <v/>
+      </c>
+      <c r="D17" t="str">
+        <v>rithvikanirvesh2909@gmail.com</v>
+      </c>
+      <c r="E17" t="str">
+        <v>08125577708</v>
+      </c>
+      <c r="F17" t="str">
+        <v/>
+      </c>
+      <c r="G17" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>AEDAKULA</v>
+      </c>
+      <c r="B18" t="str">
+        <v/>
+      </c>
+      <c r="C18" t="str">
+        <v/>
+      </c>
+      <c r="D18" t="str">
+        <v>rithvikanirvesh2909@gmail.com</v>
+      </c>
+      <c r="E18" t="str">
+        <v>08125577708</v>
+      </c>
+      <c r="F18" t="str">
+        <v/>
+      </c>
+      <c r="G18" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v/>
+      </c>
+      <c r="B19" t="str">
+        <v/>
+      </c>
+      <c r="C19" t="str">
+        <v/>
+      </c>
+      <c r="D19" t="str">
+        <v/>
+      </c>
+      <c r="E19" t="str">
+        <v/>
+      </c>
+      <c r="F19" t="str">
+        <v/>
+      </c>
+      <c r="G19" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v/>
+      </c>
+      <c r="B20" t="str">
+        <v/>
+      </c>
+      <c r="C20" t="str">
+        <v/>
+      </c>
+      <c r="D20" t="str">
+        <v/>
+      </c>
+      <c r="E20" t="str">
+        <v/>
+      </c>
+      <c r="F20" t="str">
+        <v/>
+      </c>
+      <c r="G20" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v/>
+      </c>
+      <c r="B21" t="str">
+        <v/>
+      </c>
+      <c r="C21" t="str">
+        <v/>
+      </c>
+      <c r="D21" t="str">
+        <v/>
+      </c>
+      <c r="E21" t="str">
+        <v/>
+      </c>
+      <c r="F21" t="str">
+        <v/>
+      </c>
+      <c r="G21" t="str">
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G21"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>